<commit_message>
BX9146: add field xml_id
</commit_message>
<xml_diff>
--- a/storage/app/document-templates/receipt_invoice.xlsx
+++ b/storage/app/document-templates/receipt_invoice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\romanenko_a\projects\ibt\iBT\www\ibt-oms-ms\storage\app\document-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14570DD5-4A45-4922-B272-384654E9ECA6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62847E4-A735-4F83-8F4E-3087CCF21AC1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" tabRatio="288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Поставщик:</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>2036798365661, 2036798365662</t>
+  </si>
+  <si>
+    <t>Xml ID</t>
   </si>
 </sst>
 </file>
@@ -205,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -229,12 +232,18 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -250,17 +259,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -700,48 +700,50 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="6" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="58.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="38" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
-    <col min="8" max="198" width="9.140625" style="1" customWidth="1"/>
-    <col min="199" max="16384" width="8.85546875" style="1"/>
+    <col min="3" max="4" width="16.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="58.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="38" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="1" customWidth="1"/>
+    <col min="9" max="199" width="9.140625" style="1" customWidth="1"/>
+    <col min="200" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:7" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
-    <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="12" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -751,56 +753,61 @@
       <c r="C3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="16">
+    <row r="4" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
         <v>1</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="18">
+      <c r="F4" s="11">
         <v>4</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="G4" s="18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="18">
-        <f>SUM(E4:E4)</f>
+      <c r="D5" s="3"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="11">
+        <f>SUM(F4:F4)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="6.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:7" ht="6.6" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="3">
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
-  <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="83" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <headerFooter alignWithMargins="0"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="63" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>